<commit_message>
add graphAnalysis LoadData ,RenameTab,QueryLoadStatus case
</commit_message>
<xml_diff>
--- a/src/main/resources/data/addGraph-test.xlsx
+++ b/src/main/resources/data/addGraph-test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28000" windowHeight="12500"/>
+    <workbookView windowWidth="28000" windowHeight="13120"/>
   </bookViews>
   <sheets>
     <sheet name="工作表 1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17">
   <si>
     <t>title</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>expectMessage</t>
+  </si>
+  <si>
+    <t>isRun</t>
   </si>
   <si>
     <t>图分析视图-addGraph-成功新增标签页</t>
@@ -56,6 +59,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
       <t>图分析视图</t>
     </r>
     <r>
@@ -128,6 +138,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="宋体-简"/>
+        <charset val="134"/>
+      </rPr>
       <t>图分析视图</t>
     </r>
     <r>
@@ -157,10 +174,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -198,6 +215,35 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Helvetica Neue"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -211,10 +257,34 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -226,23 +296,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,47 +349,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
       <name val="Helvetica Neue"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -310,43 +364,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -375,13 +392,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -393,13 +548,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,85 +560,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,61 +572,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -647,19 +664,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -673,17 +679,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -699,21 +699,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -735,9 +720,41 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -746,148 +763,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -936,55 +953,55 @@
     </xf>
   </cellXfs>
   <cellStyles count="49">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
-    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
-    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
-    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
-    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
-    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
-    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
-    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
-    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
-    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
-    <cellStyle name="40% - Accent1" xfId="17" builtinId="31"/>
-    <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
-    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
-    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
-    <cellStyle name="Bad" xfId="22" builtinId="27"/>
-    <cellStyle name="20% - Accent4" xfId="23" builtinId="42"/>
-    <cellStyle name="Total" xfId="24" builtinId="25"/>
-    <cellStyle name="Output" xfId="25" builtinId="21"/>
-    <cellStyle name="Currency" xfId="26" builtinId="4"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
-    <cellStyle name="Note" xfId="28" builtinId="10"/>
-    <cellStyle name="Input" xfId="29" builtinId="20"/>
-    <cellStyle name="Heading 4" xfId="30" builtinId="19"/>
-    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
-    <cellStyle name="Good" xfId="32" builtinId="26"/>
-    <cellStyle name="Heading 3" xfId="33" builtinId="18"/>
-    <cellStyle name="CExplanatory Text" xfId="34" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
-    <cellStyle name="Comma [0]" xfId="36" builtinId="6"/>
-    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
-    <cellStyle name="Title" xfId="38" builtinId="15"/>
-    <cellStyle name="Currency [0]" xfId="39" builtinId="7"/>
-    <cellStyle name="Warning Text" xfId="40" builtinId="11"/>
-    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9"/>
-    <cellStyle name="20% - Accent2" xfId="42" builtinId="34"/>
-    <cellStyle name="Link" xfId="43" builtinId="8"/>
-    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
-    <cellStyle name="Comma" xfId="45" builtinId="3"/>
-    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
-    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
-    <cellStyle name="Percent" xfId="48" builtinId="5"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
   <tableStyles count="0"/>
   <colors>
@@ -2106,7 +2123,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="E1" sqref="E1:E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3303571428571" defaultRowHeight="19.9" customHeight="1" outlineLevelCol="5"/>
@@ -2131,73 +2148,85 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3"/>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="F1" s="3"/>
     </row>
     <row r="2" ht="20.25" customHeight="1" spans="1:6">
       <c r="A2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
-      <c r="E2" s="13"/>
+      <c r="E2" s="13">
+        <v>1</v>
+      </c>
       <c r="F2" s="13"/>
     </row>
     <row r="3" ht="20.05" customHeight="1" spans="1:6">
       <c r="A3" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="E3" s="9">
+        <v>0</v>
+      </c>
       <c r="F3" s="9"/>
     </row>
     <row r="4" ht="20.05" customHeight="1" spans="1:6">
       <c r="A4" s="8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="10">
         <v>201</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="E4" s="9">
+        <v>0</v>
+      </c>
       <c r="F4" s="9"/>
     </row>
     <row r="5" ht="20.05" customHeight="1" spans="1:6">
       <c r="A5" s="8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="9"/>
       <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="E5" s="9">
+        <v>0</v>
+      </c>
       <c r="F5" s="9"/>
     </row>
     <row r="6" ht="20.05" customHeight="1" spans="1:6">
       <c r="A6" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="E6" s="9">
+        <v>0</v>
+      </c>
       <c r="F6" s="9"/>
     </row>
     <row r="7" ht="20.05" customHeight="1" spans="1:6">

</xml_diff>